<commit_message>
updated example_script_matlab, added in separate reference files for terminators and spacers
</commit_message>
<xml_diff>
--- a/example_ref_sequences/100k_Terminators.xlsx
+++ b/example_ref_sequences/100k_Terminators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab Users\ROC\20220530_Exp54-100kBigBird_Part1\Outputs\pass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\OneDrive\Documents\GitHub\WIMPY\example_ref_sequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D026A5-4CA5-4151-BB25-481C8F5D1F6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08575D87-30FF-4EE9-975A-7E123DB38803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="8415" xr2:uid="{DEDAC577-AF37-4D1E-B94C-332B72315728}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DEDAC577-AF37-4D1E-B94C-332B72315728}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Sequence</t>
   </si>
@@ -36,73 +36,25 @@
     <t>SV40</t>
   </si>
   <si>
-    <t>SV40 + 250bp</t>
-  </si>
-  <si>
-    <t>SV40 + 500bp</t>
-  </si>
-  <si>
     <t>bGH225</t>
   </si>
   <si>
-    <t>bGH225 + 250bp</t>
-  </si>
-  <si>
-    <t>bGH225 + 500bp</t>
-  </si>
-  <si>
     <t>sT1A18</t>
   </si>
   <si>
-    <t>sT1A18 + 250bp</t>
-  </si>
-  <si>
-    <t>sT1A18 + 500bp</t>
-  </si>
-  <si>
     <t>T1A9</t>
   </si>
   <si>
-    <t>T1A9 + 250bp</t>
-  </si>
-  <si>
-    <t>T1A9 + 500bp</t>
-  </si>
-  <si>
-    <t>AACTTGTTTATTGCAGCTTATAATGGTTACAAATAAAGCAATAGCATCACAAATTTCACAAATAAAGCATTTTTTTCACTGCATTCTAGTTGTGGTTTGTCCAAACTCATCAATGTATCTTATCATGTCTGCCCATGATAGGGGATCTGTGAGATGGGTGTGTATAGATCTTTGGCCATATCTGAGAGTCTGGTTGGGTTCCATTTGTAGAGCCTGACCTTTAAGAATGTGTCAGAGACTGGTGTCTAAGCCCGCTAAGGCCTAAACAAGTGAATCTTTTGAATCTCTCTTTTTTTTTTTTGAGACAGAGTCTTGTTCTGTCACCCAGGCTGGAGTGCAGTGGTATGATCTCGGCTCACTGCAACTCCTGCCTTCCAGGTTCAAGC</t>
-  </si>
-  <si>
     <t>ctgtgccttctagttgccagccatctgttgtttgcccctcccccgtgccttccttgaccctggaaggtgccactcccactgtcctttcctaataaaatgaggaaattgcatcgcattgtctgagtaggtgtcattctattctggggggtggggtggggcaggacagcaagggggaggattgggaaggcaatagcaggcatgctggggatgcggtgggctctatgg</t>
   </si>
   <si>
-    <t>CCATATCTTGGAGGGAGAGTAGGTATTTGTGATTTGTGTATTATTTTAATAAAGGTTTTATGACACATGTTCGCTATTCCGCACGTCGGCCGCCGATGAATAAAGTCCTGCCCGGTCGGCTTGAGTGCGTGTGTCTCGTTTAGATGCTGCGCCTAACCCTAAGCAGATTCTTCATGCAACCATGATAGGGGATCTGTGAGATGGGTGTGTATAGATCTTTGGCCATATCTGAGAGTCTGGTTGGGTTCCATTTGTAGAGCCTGACCTTTAAGAATGTGTCAGAGACTGGTGTCTAAGCCCGCTAAGGCCTAAACAAGTGAATCTTTTGAATCTCTCTTTTTTTTTTTTGAGACAGAGTCTTGTTCTGTCACCCAGGCTGGAGTGCAGTGGTATGATCTCGGCTCACTGCAACTCCTGCCTTCCAGGTTCAAGC</t>
-  </si>
-  <si>
-    <t>CCATATCTTTTGGACTGGGACGCGGGATTCTTACCAATGCTTTGTGTAAATAAATATTTATCCCCGATTCAACCCACAATAGCCTTCACACCCATCGGTGCCAAAATAAAGTCCTGCCCGGTCGGCTTGAGTGCGTGTGTCTCGTTTAGATGCTGCGCCTAACCCTAAGCAGATTCTTCACCATGATAGGGGATCTGTGAGATGGGTGTGTATAGATCTTTGGCCATATCTGAGAGTCTGGTTGGGTTCCATTTGTAGAGCCTGACCTTTAAGAATGTGTCAGAGACTGGTGTCTAAGCCCGCTAAGGCCTAAACAAGTGAATCTTTTGAATCTCTCTTTTTTTTTTTTGAGACAGAGTCTTGTTCTGTCACCCAGGCTGGAGTGCAGTGGTATGATCTCGGCTCACTGCAACTCCTGCCTTCCAGGTTCAAGC</t>
-  </si>
-  <si>
     <t>atcttttggactgggacgcgggattcttaccaatgctttgtgtaaataaatatttatccccgattcaacccacaatagccttcacacccatcggtgccaaaataaagtcctgcccggtcggcttgagtgcgtgtgtctcgtttagatgctgcgcctaaccctaagcagattcttca</t>
   </si>
   <si>
-    <t>CTGTGCCTTCTAGTTGCCAGCCATCTGTTGTTTGCCCCTCCCCCGTGCCTTCCTTGACCCTGGAAGGTGCCACTCCCACTGTCCTTTCCTAATAAAATGAGGAAATTGCATCGCATTGTCTGAGTAGGTGTCATTCTATTCTGGGGGGTGGGGTGGGGCAGGACAGCAAGGGGGAGGATTGGGAAGGCAATAGCAGGCATGCTGGGGATGCGGTGGGCTCTATGGCCATGATAGGGGATCTGTGAGATGGGTGTGTATAGATCTTTGGCCATATCTGAGAGTCTGGTTGGGTTCCATTTGTAGAGCCTGACCTTTAAGAATGTGTCAGAGACTGGTGTCTAAGCCCGCTAAGGCCTAAACAAGTGAATCTTTTGAATCTCTCTTTTTTTTTTTTGAGACAGAGTCTTGTTCTGTCACCCAGGCTGGAGTGCAGTGGTATGATCTCGGCTCACTGCAACTCCTGCCTTCCAGGTTCAAGC</t>
-  </si>
-  <si>
-    <t>CCATATCTTGGAGGGAGAGTAGGTATTTGTGATTTGTGTATTATTTTAATAAAGGTTTTATGACACATGTTCGCTATTCCGCACGTCGGCCGCCGATGAATAAAGTCCTGCCCGGTCGGCTTGAGTGCGTGTGTCTCGTTTAGATGCTGCGCCTAACCCTAAGCAGATTCTTCATGCAACCATGATAGGGGATCTGTGAGATGGGTGTGTATAGATCTTTGGCCATATCTGAGAGTCTGGTTGGGTTCCATTTGTAGAGCCTGACCTTTAAGAATGTGTCAGAGACTGGTGTCTAAGCCCGCTAAGGCCTAAACAAGTGAATCTTTTGAATCTCTCTTTTTTTTTTTTGAGACAGAGTCTTGTTCTGTCACCCAGGCTGGAGTGCAGTGGTATGATCTCGGCTCACTGCAACTCCTGCCTTCCAGGTTCAAGCAATTCTCCTTCCTCAGCCTCCCAAGTAGCTGGGATTACAGGCACTTGCCATCATGCCTGTCTAATTTTTGTATTTTTGTAGAGATGGGATTTCACCATGTTGGCCAGGTTGGTCTTGAACTCTTGACCTCAGGTGATCTGCCTGCCTTGGCCTCCCAAAATTCTGGGATTACAGGCGTGAGCCACCACTCCCAGCCTCTAAACAAGTGAATCTTAATTGCTCCTCCTCAGACTAAGGAATATCTAGGATC</t>
-  </si>
-  <si>
-    <t>CCATATCTTTTGGACTGGGACGCGGGATTNTTACCAATGCTTTGTGTAAATAAATATTTATCCCCGATTCAACCCACAATAGCCTTCACACCCATCGGTGCCAAAATAAAGTCCTGCCCGGTCGGCTTGAGTGCGTGTGTCTCGTTTAGATGCTGCGCCTAACCCTAAGCAGATTCTTCACCATGATAGGGGATCTGTGAGATGGGTGTGTATAGATCTTTGGCCATATCTGAGAGTCTGGTTGGGTTCCATTTGTAGAGCCTGACCTTTAAGAATGTGTCAGAGACTGGTGTCTAAGCCCGCTAAGGCCTAAACAAGTGAATCTTTTGAATCTCTCTTTTTTTTTTTTGAGACAGAGTCTTGTTCTGTCACCCAGGCTGGAGTGCAGTGGTATGATCTCGGCTCACTGCAACTCCTGCCTTCCAGGTTCAAGCAATTCTCCTTCCTCAGCCTCCCAAGTAGCTGGGATTACAGGCACTTGCCATCATGCCTGTCTAATTTTTGTATTTTTGTAGAGATGGGATTTCACCATGTTGGCCAGGTTGGTCTTGAACTCTTGACCTCAGGTGATCTGCCTGCCTTGGCCTCCCAAAATTCTGGGATTACAGGCGTGAGCCACCACTCCCAGCCTCTAAACAAGTGAATCTTAATTGCTCCTCCTCAGACTAAGGAATATCTAGGATC</t>
-  </si>
-  <si>
     <t>AACTTGTTTATTGCAGCTTATAATGGTTACAAATAAAGCAATAGCATCACAAATTTCACAAATAAAGCATTTTTTTCACTGCATTCTAGTTGTGGTTTGTCCAAACTCATCAATGTATCTTATCATGTCTG</t>
   </si>
   <si>
     <t>ccatatcttggagggagagtaggtatttgtgatttgtgtattattttaataaaggttttatgacacatgttcgctattccgcacgtcggccgccgatgaataaagtcctgcccggtcggcttgagtgcgtgtgtctcgtttagatgctgcgcctaaccctaagcagattcttcatgcaa</t>
-  </si>
-  <si>
-    <t>AACTTGTTTATTGCAGCTTATAATGGTTACAAATAAAGCAATAGCATCACAAATTTCACAAATAAAGCATTTTTTTCACTGCATTCTAGTTGTGGTTTGTCCAAACTCATCAATGTATCTTATCATGTCTGCCCATGATAGGGGATTGTGAGATGGGTGTGTATAGATCTTTGGCCATATCTGAGAGTCTGGTTGGGTTCCATTTGTAGAGCCTGACCTTTAAGAATGTGTCAGAGACTGGTGTCTAAGCCCGCTAAGGCCTAAACAAGTGAATCTTTTGAATCTCTCTTTTTTTTTTTTGAGACAGAGTCTTGTTCTGTCACCCAGGCTGGAGTGCAGTGGTATGATCTCGGCTCACTGCAACTCCTGCCTTCCAGGTTCAAGCAATTCTCCTTCCTCAGCCTCCCAAGTAGCTGGGATTACAGGCACTTGCCATCATGCCTGTCTAATTTTTGTATTTTTGTAGAGATGGGATTTCACCATGTTGGCCAGGTTGGTCTTGAACTCTTGACCTCAGGTGATCTGCCTGCCTTGGCCTCCCAAAATTCTGGGATTACAGGCGTGAGCCACCACTCCCAGCCTCTAAACAAGTGAATCTTAATTGCTCCTCCTCAGACTAAGGAATATCTAGGATC</t>
-  </si>
-  <si>
-    <t>ctgtgccttctagttgccagccatctgttgtttgcccctcccccgtgccttccttgaccctggaaggtgccactcccactgtcctttcctaataaaatgaggaaattgcatcgcattgtctgagtaggtgtcattctattctggggggtggggtggggcaggacagcaagggggaggattgggaaggcaatagcaggcatgctggggatgcggtgggctctatggCCATgataggggatctgtgagatgggtgtgtatagatctttggccatatctgagagtctggttgggttccatttgtagagcctgacctttaagaatgtgtcagagactggtgtctaagcccgctaaggcctaaacaagtgaatcttttgaatctctcttttttttttttgagacagagtcttgttctgtcacccaggctggagtgcagtggtatgatctcggctcactgcaactcctgccttccaggttcaagcaattctccttcctcagcctcccaagtagctgggattacaggcacttgccatcatgcctgtctaatttttgtatttttgtagagatgggatttcaccatgttggccaggttggtcttgaactcttgacctcaggtgatctgcctgccttggcctcccaaaattctgggattacaggcgtgagccaccactcccagcctctaaacaagtgaatcttaattgctcctcctcagactaaggaatatctaggatc</t>
   </si>
 </sst>
 </file>
@@ -167,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -207,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -313,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -455,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -463,20 +415,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FC080B-1C35-4F84-A21E-2E16EBA62D5A}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -485,100 +437,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
         <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>